<commit_message>
Adicionada a foto do diagrama de ER
</commit_message>
<xml_diff>
--- a/src/assets/planilhas/xlsx/circuitos.xlsx
+++ b/src/assets/planilhas/xlsx/circuitos.xlsx
@@ -1020,10 +1020,10 @@
     <t>pais</t>
   </si>
   <si>
-    <t>long</t>
-  </si>
-  <si>
     <t>cidade</t>
+  </si>
+  <si>
+    <t>lng</t>
   </si>
 </sst>
 </file>
@@ -1871,7 +1871,7 @@
   <dimension ref="A1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1895,7 +1895,7 @@
         <v>331</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>332</v>
@@ -1904,7 +1904,7 @@
         <v>323</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>249</v>

</xml_diff>